<commit_message>
Carrito y entrada de datos
se agregaron entradas de datos se modificaron los archivos html css y js para la entrada de multiples paginas de excel
</commit_message>
<xml_diff>
--- a/Tienda/datasheet productos.xlsx
+++ b/Tienda/datasheet productos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rar/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rar/Documents/GitHub/GameofGrow/Tienda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E2951C3-302F-E54E-8EEE-8AC724DA827E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0F0A1D-0F33-A246-8DCC-C0EA86D2CA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="13160" windowHeight="15800" xr2:uid="{F81F158D-7208-714E-A214-AAFC90E62AF1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{F81F158D-7208-714E-A214-AAFC90E62AF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Semillas" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -148,6 +148,54 @@
   </si>
   <si>
     <t>Marca</t>
+  </si>
+  <si>
+    <t>Kit indoor 60</t>
+  </si>
+  <si>
+    <t>Kit indoor 80</t>
+  </si>
+  <si>
+    <t>Kit indoor 100</t>
+  </si>
+  <si>
+    <t>Ligth mix</t>
+  </si>
+  <si>
+    <t>Biobuzz</t>
+  </si>
+  <si>
+    <t>All mix</t>
+  </si>
+  <si>
+    <t>Top crop</t>
+  </si>
+  <si>
+    <t>Microrizas</t>
+  </si>
+  <si>
+    <t>pack semillas</t>
+  </si>
+  <si>
+    <t>GameofGrow</t>
+  </si>
+  <si>
+    <t>Wonderland</t>
+  </si>
+  <si>
+    <t>Oferta</t>
+  </si>
+  <si>
+    <t>Sustrato</t>
+  </si>
+  <si>
+    <t>ocb negros</t>
+  </si>
+  <si>
+    <t>Ocb</t>
+  </si>
+  <si>
+    <t>Papelillo</t>
   </si>
 </sst>
 </file>
@@ -514,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0FA759-ED61-254E-A261-DB59E703099C}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,10 +863,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DDBC011-ECAB-D44C-9527-555B32369049}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,6 +892,236 @@
       </c>
       <c r="G1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>150000</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>200000</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>20000</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>23000</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>23000</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8">
+        <v>25000</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>5000</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10">
+        <v>15000</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>